<commit_message>
update inputs and ignored them
</commit_message>
<xml_diff>
--- a/public/simple-data/v3.antpool.comhome2.xlsx
+++ b/public/simple-data/v3.antpool.comhome2.xlsx
@@ -5,25 +5,24 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali\Documents\GitHub\Crypto-Currencies-Card---table\public\simple-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Crypto-Currencies-Card---table\public\simple-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$H$206</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$F$206</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="225">
   <si>
     <t>Whatsminer M30S++</t>
   </si>
@@ -698,32 +697,19 @@
   </si>
   <si>
     <t>K</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>th</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF1A01CC"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -746,7 +732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -754,7 +740,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1094,23 +1079,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H206"/>
+  <dimension ref="A1:F206"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="G1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.25" customWidth="1"/>
-    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="11.125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>215</v>
       </c>
@@ -1129,14 +1114,8 @@
       <c r="F1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="G1">
-        <v>110</v>
-      </c>
-      <c r="H1" s="3">
-        <v>266549</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1156,7 +1135,7 @@
         <v>3472</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1176,7 +1155,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1196,7 +1175,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1216,7 +1195,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1236,7 +1215,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1256,7 +1235,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1276,7 +1255,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1296,7 +1275,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1316,7 +1295,7 @@
         <v>3420</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1336,7 +1315,7 @@
         <v>3344</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1356,7 +1335,7 @@
         <v>3230</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1376,7 +1355,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1396,7 +1375,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1416,7 +1395,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1436,7 +1415,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1456,7 +1435,7 @@
         <v>3276</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1476,7 +1455,7 @@
         <v>3432</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1496,7 +1475,7 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1516,7 +1495,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1536,7 +1515,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1556,7 +1535,7 @@
         <v>2920</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1576,7 +1555,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1596,7 +1575,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1616,7 +1595,7 @@
         <v>3312</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1636,7 +1615,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1656,7 +1635,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1676,7 +1655,7 @@
         <v>2680</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1696,7 +1675,7 @@
         <v>3260</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1716,7 +1695,7 @@
         <v>3312</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1736,7 +1715,7 @@
         <v>3325</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1756,7 +1735,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1776,7 +1755,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1796,7 +1775,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1816,7 +1795,7 @@
         <v>3350</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1836,7 +1815,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1856,7 +1835,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1876,7 +1855,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1896,7 +1875,7 @@
         <v>3276</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1916,7 +1895,7 @@
         <v>3276</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1936,7 +1915,7 @@
         <v>2976</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1956,7 +1935,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1976,7 +1955,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1996,7 +1975,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2016,7 +1995,7 @@
         <v>3348</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2036,7 +2015,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2056,7 +2035,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2076,7 +2055,7 @@
         <v>3480</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2096,7 +2075,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2116,7 +2095,7 @@
         <v>2094</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2136,7 +2115,7 @@
         <v>3505</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2156,7 +2135,7 @@
         <v>2385</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2176,7 +2155,7 @@
         <v>3340</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2196,7 +2175,7 @@
         <v>3340</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2216,7 +2195,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2236,7 +2215,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2256,7 +2235,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2276,7 +2255,7 @@
         <v>3240</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2296,7 +2275,7 @@
         <v>2915</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2316,7 +2295,7 @@
         <v>3575</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2336,7 +2315,7 @@
         <v>3445</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2356,7 +2335,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2376,7 +2355,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2396,7 +2375,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2416,7 +2395,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2436,7 +2415,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2456,7 +2435,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2476,7 +2455,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2496,7 +2475,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2516,7 +2495,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2536,7 +2515,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2556,7 +2535,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2576,7 +2555,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -2596,7 +2575,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -2616,7 +2595,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -2636,7 +2615,7 @@
         <v>2508</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -2656,7 +2635,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -2676,7 +2655,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -2696,7 +2675,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -2716,7 +2695,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -2736,7 +2715,7 @@
         <v>2405</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -2756,7 +2735,7 @@
         <v>6400</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -2776,7 +2755,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -2796,7 +2775,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -2816,7 +2795,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -2836,7 +2815,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -2856,7 +2835,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -2876,7 +2855,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -2896,7 +2875,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -2916,7 +2895,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -2936,7 +2915,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -2956,7 +2935,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -2976,7 +2955,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -2996,7 +2975,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -3016,7 +2995,7 @@
         <v>1541</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -3036,7 +3015,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -3056,7 +3035,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -3076,7 +3055,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -3096,7 +3075,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -3116,7 +3095,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -3136,7 +3115,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -3156,7 +3135,7 @@
         <v>1530</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -3176,7 +3155,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -3196,7 +3175,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -3216,7 +3195,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -3236,7 +3215,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -3256,7 +3235,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -3276,7 +3255,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -3296,7 +3275,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -3316,7 +3295,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -3336,7 +3315,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -3356,7 +3335,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -3376,7 +3355,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -3396,7 +3375,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -3416,7 +3395,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -3436,7 +3415,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -3456,7 +3435,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -3476,7 +3455,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -3496,7 +3475,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -3516,7 +3495,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -3536,7 +3515,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -3556,7 +3535,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -3576,7 +3555,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -3596,7 +3575,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -3616,7 +3595,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -3636,7 +3615,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -3656,7 +3635,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -3676,7 +3655,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -3696,7 +3675,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -3716,7 +3695,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -3736,7 +3715,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -3756,7 +3735,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -3776,7 +3755,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -4056,7 +4035,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -4076,7 +4055,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -4096,7 +4075,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -4116,7 +4095,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -4136,7 +4115,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -4156,7 +4135,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -4176,7 +4155,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -4196,7 +4175,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -4216,7 +4195,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -4236,7 +4215,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -4256,7 +4235,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -4276,7 +4255,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -4296,7 +4275,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -4316,7 +4295,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -4336,7 +4315,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -4356,7 +4335,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -4376,7 +4355,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -4396,7 +4375,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -4416,7 +4395,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -4436,7 +4415,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -4456,7 +4435,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -4476,7 +4455,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -4496,7 +4475,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -4516,7 +4495,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -4536,7 +4515,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -4556,7 +4535,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -4576,7 +4555,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -4596,7 +4575,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -4616,7 +4595,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -4636,7 +4615,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -4656,7 +4635,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -4676,7 +4655,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -4696,7 +4675,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -4716,7 +4695,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -4736,7 +4715,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -4756,7 +4735,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -4776,7 +4755,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -4796,7 +4775,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -4816,7 +4795,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -4836,7 +4815,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -4856,7 +4835,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -4876,7 +4855,7 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -4896,7 +4875,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -4916,7 +4895,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -4936,7 +4915,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -4956,7 +4935,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -4976,7 +4955,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -4996,7 +4975,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -5016,7 +4995,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -5036,7 +5015,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -5056,7 +5035,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -5076,7 +5055,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -5096,7 +5075,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -5116,7 +5095,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -5136,7 +5115,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -5156,7 +5135,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -5176,7 +5155,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -5196,7 +5175,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -5216,7 +5195,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -5237,76 +5216,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H206">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="ETH"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F206"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <ignoredErrors>
     <ignoredError sqref="F207:F209 B2:C206 C207 B208:C209" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>112</v>
-      </c>
-      <c r="C3">
-        <v>3472</v>
-      </c>
-      <c r="D3">
-        <v>1255.6600000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4">
-        <v>1841</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>110</v>
-      </c>
-      <c r="B10" s="3">
-        <v>266549</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <f>43.17*30</f>
-        <v>1295.1000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f>A10/B10</f>
-        <v>4.1268209597484888E-4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>